<commit_message>
created a relationship for the ReadFromFile and PurchaseProductsTest classes
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5C6C62-3A83-4F0D-ACA6-148961B35B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Added classes on Read file to read infomation values Added infomation page elements and methods
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\uh09200086.bmwgroup.net\home$\QXZ47OH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B04927-211F-4BBA-8366-3C88D2B607E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -44,6 +44,21 @@
   </si>
   <si>
     <t>invalid_password</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name </t>
+  </si>
+  <si>
+    <t>ZIP/Postal Code</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>June</t>
   </si>
 </sst>
 </file>
@@ -386,17 +401,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -412,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -420,33 +435,62 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"BMW Group Condensed"&amp;12&amp;KC00000 CONFIDENTIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"BMW Group Condensed"&amp;12&amp;KC00000 CONFIDENTIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added user details to excel sheet2
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\automation class 2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="user_details" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -44,12 +43,27 @@
   </si>
   <si>
     <t>invalid_password</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Ree</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,11 +397,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,15 +452,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new classes for data and read from a file. and Addent the methods on the purchaseproduct test also added the xl file
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmahinga.TRACKER\AutomationProject\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27031CC-A24C-4DD7-8758-A2ED5E14EB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="user_details" sheetId="2" r:id="rId2"/>
+    <sheet name="CheckoutDetails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,24 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Username</t>
+    <t>FirstName</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>LastName</t>
   </si>
   <si>
-    <t>standard_user</t>
+    <t>PostalCode</t>
   </si>
   <si>
-    <t>secret_sauce</t>
+    <t>Selina</t>
   </si>
   <si>
-    <t>Wrong_user</t>
-  </si>
-  <si>
-    <t>invalid_password</t>
+    <t>Mayinga</t>
   </si>
 </sst>
 </file>
@@ -68,7 +64,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -102,8 +98,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,69 +380,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6500</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new classes for data and read from a file. and Addent the methods on the purchaseproduct test also added the xl file and added new method
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmahinga.TRACKER\AutomationProject\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DB05C2-C449-4645-8611-E9CFE8D9DC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03588B65-C040-429C-A25F-EB2877377F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3144" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckoutDetails" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
created read from file values
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationProject\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2F8FCF-244E-4B1E-B64E-DE18729CCB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -44,6 +44,27 @@
   </si>
   <si>
     <t>invalid_password</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Postalcode</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Khulekani</t>
+  </si>
+  <si>
+    <t>Hlengwa</t>
+  </si>
+  <si>
+    <t>Mlungu</t>
+  </si>
+  <si>
+    <t>Wamodimo</t>
   </si>
 </sst>
 </file>
@@ -386,17 +407,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -412,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -420,15 +441,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
@@ -439,14 +460,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>36845</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>33502</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add data from excel,ReadFromFile and YourInfoPage
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationProjects\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDEC2E0-F500-4D73-911D-FDB94B6F614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t>invalid_password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName </t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Neon</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
 </sst>
 </file>
@@ -59,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,6 +87,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -100,10 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,17 +412,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -412,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -420,15 +446,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
@@ -439,14 +465,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created a class ReadFromFile reading data from excel file fort he Loging page and Checkout: Your Information Page
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationProjects\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AE00F6-A201-4C6D-9707-25BAD72C1B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -44,6 +44,21 @@
   </si>
   <si>
     <t>invalid_password</t>
+  </si>
+  <si>
+    <t>Tami</t>
+  </si>
+  <si>
+    <t>Tam</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Zip/Postal Code</t>
   </si>
 </sst>
 </file>
@@ -386,17 +401,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -412,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -420,15 +435,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
@@ -439,14 +454,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2121</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
We combined Amanda_playground's code with the main branch code
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D35652-9D84-4335-9E1A-46BF78FA12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="user_details" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -40,16 +30,31 @@
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>Wrong_user</t>
-  </si>
-  <si>
-    <t>invalid_password</t>
+    <t>Wrong_use</t>
+  </si>
+  <si>
+    <t>Wrong_password</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Ramavhale</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,7 +73,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -100,16 +105,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -132,44 +138,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -199,12 +205,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -243,209 +249,262 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1632</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23C21B-9522-4AF0-9490-AEE85FFC8B19}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added read from a file for a check out page.added new code
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmahinga.TRACKER\AutomationProject\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6819AFCD-A439-4C62-96E6-774638DF46DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B90E3CD-CFAD-4942-ACDB-4FC9E37AE820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3144" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2388" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckoutDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,21 +26,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>PostalCode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Selina</t>
   </si>
   <si>
     <t>Mayinga</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Postalcode</t>
+  </si>
+  <si>
+    <t>6500</t>
   </si>
 </sst>
 </file>
@@ -64,7 +68,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,10 +100,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,7 +390,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,38 +401,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>6500</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E4BCC6-DB6D-4231-8EEC-B2727CB82C2F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created the whole thing
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationProject\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2F8FCF-244E-4B1E-B64E-DE18729CCB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5B2626-1C63-4F93-9155-2FCC23493386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Wamodimo</t>
+  </si>
+  <si>
+    <t>36845</t>
+  </si>
+  <si>
+    <t>33502</t>
   </si>
 </sst>
 </file>
@@ -121,10 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +470,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,8 +498,8 @@
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
-        <v>36845</v>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,8 +509,8 @@
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
-        <v>33502</v>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated clickcart method in cartpage
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView windowWidth="20130" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="user_details" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,12 +49,6 @@
     <t>Wrong_password</t>
   </si>
   <si>
-    <t>Amanda</t>
-  </si>
-  <si>
-    <t>Ramavhale</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -50,21 +57,184 @@
   <si>
     <t>PostalCode</t>
   </si>
+  <si>
+    <t>neo</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,8 +247,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -88,43 +444,335 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,25 +1056,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="A1" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="18.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -442,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -452,60 +1100,67 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1632</v>
+      <c r="C2" s="2">
+        <v>1939</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted and Added New classes. added more code on the created classes
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmahinga.TRACKER\AutomationProject\SauceDemo3rdGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066E2E4C-E21D-4783-B424-7FC8E37C754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8BF4C9-7F7E-4ED2-87C8-FFE0595F1770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2388" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2388" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="user_details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +41,21 @@
   </si>
   <si>
     <t>problem_user</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Postalcode</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Selina</t>
+  </si>
+  <si>
+    <t>Mabunda</t>
   </si>
 </sst>
 </file>
@@ -382,7 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -419,4 +435,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AFA77A1-B04A-416F-838F-58B1841364C6}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>